<commit_message>
Document Structure change, Added Demo slides
</commit_message>
<xml_diff>
--- a/Documents/Sprint Planning/Sprint Logs.xlsx
+++ b/Documents/Sprint Planning/Sprint Logs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/Sprint Planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT\Documents\Sprint Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{58AE748A-8CE0-4192-BA4A-FDA7D93F3733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68A0E1CC-5522-4433-A04F-C362C5978FF2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19728FB0-29C7-4486-9F68-C65DC28CD7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="-3630" windowWidth="19200" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="269">
   <si>
     <t>Location</t>
   </si>
@@ -1024,6 +1024,10 @@
   </si>
   <si>
     <t>Submitted Final Report</t>
+  </si>
+  <si>
+    <t>Proofread the report
+Make final changes to logs</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1181,6 +1185,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1488,8 +1495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4054,11 +4061,13 @@
         <v>264</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="16">
         <v>45406</v>
       </c>
-      <c r="B101" s="19"/>
+      <c r="B101" s="12" t="s">
+        <v>158</v>
+      </c>
       <c r="C101" s="12" t="s">
         <v>15</v>
       </c>
@@ -4068,18 +4077,39 @@
       <c r="E101" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F101" s="19" t="s">
+      <c r="F101" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G101" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="9"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="16">
+        <v>45407</v>
+      </c>
+      <c r="B102" s="29">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="G101" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H101" s="9" t="s">
+      <c r="G102" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H102" s="9" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H102" s="10"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H103" s="10"/>

</xml_diff>